<commit_message>
agrego tabla de routers con ip y cambie el de subredes proque al parecer habia subido una versin vieja
</commit_message>
<xml_diff>
--- a/ tp-distribuidos-grupo3/Tabla de subredes - Subnetting.xlsx
+++ b/ tp-distribuidos-grupo3/Tabla de subredes - Subnetting.xlsx
@@ -739,9 +739,9 @@
   <cols>
     <col min="1" customWidth="1" max="1" width="3.57"/>
     <col min="3" customWidth="1" max="3" width="10.71"/>
-    <col min="4" customWidth="1" max="4" hidden="1" width="24.0"/>
-    <col min="5" customWidth="1" max="5" hidden="1" width="30.57"/>
-    <col min="6" customWidth="1" max="6" hidden="1" width="10.0"/>
+    <col min="4" customWidth="1" max="4" width="24.0"/>
+    <col min="5" customWidth="1" max="5" width="30.57"/>
+    <col min="6" customWidth="1" max="6" width="10.0"/>
     <col min="7" customWidth="1" max="7" width="16.86"/>
     <col min="8" customWidth="1" max="8" width="21.0"/>
   </cols>

</xml_diff>

<commit_message>
Cambio R9 a Sede El Calafate
</commit_message>
<xml_diff>
--- a/ tp-distribuidos-grupo3/Tabla de subredes - Subnetting.xlsx
+++ b/ tp-distribuidos-grupo3/Tabla de subredes - Subnetting.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="390" yWindow="540" windowWidth="18615" windowHeight="5835"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="132">
   <si>
     <t>Red</t>
   </si>
@@ -275,9 +278,6 @@
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>??</t>
   </si>
   <si>
     <t>Giant</t>
@@ -415,68 +415,46 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF6AA84F"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <i/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
       <i/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -486,9 +464,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -678,737 +654,1033 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="2" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="3" applyFont="1" fontId="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="4" applyFont="1" fontId="2">
-      <alignment vertical="bottom" horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="5" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="6" applyFont="1" fontId="3">
-      <alignment vertical="bottom" horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="7" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="8" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="9" applyFont="1" fontId="4">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="10" applyFont="1" fontId="5" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="11" fontId="0">
-      <alignment vertical="bottom" horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="12" applyFont="1" fontId="6">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="13" fontId="0">
-      <alignment vertical="bottom" horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="3.57"/>
-    <col min="3" customWidth="1" max="3" width="10.71"/>
-    <col min="4" customWidth="1" max="4" width="24.0"/>
-    <col min="5" customWidth="1" max="5" width="30.57"/>
-    <col min="6" customWidth="1" max="6" width="10.0"/>
-    <col min="7" customWidth="1" max="7" width="16.86"/>
-    <col min="8" customWidth="1" max="8" width="21.0"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="10" r="A1">
+    <row r="1" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="10" r="B1">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="10" r="C1">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="10" r="D1">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="10" r="E1">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="10" r="F1">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="10" r="G1">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="10" r="H1">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c s="1" r="I1"/>
-    </row>
-    <row r="2">
-      <c t="s" s="3" r="A2">
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="2" r="B2">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="2" r="C2">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="2" r="D2">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="13" r="E2">
+      <c r="E2" s="13" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="13" r="F2">
+      <c r="F2" s="13" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="6" r="G2">
+      <c r="G2" s="6" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="4" r="H2">
+      <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
-      <c s="1" r="I2"/>
-    </row>
-    <row r="3">
-      <c t="s" s="3" r="A3">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="9" r="B3">
+      <c r="B3" s="9" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="2" r="C3">
+      <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
-      <c t="s" s="2" r="D3">
+      <c r="D3" s="2" t="s">
         <v>19</v>
       </c>
-      <c s="13" r="E3">
+      <c r="E3" s="13">
         <v>5</v>
       </c>
-      <c t="s" s="13" r="F3">
+      <c r="F3" s="13" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="6" r="G3">
+      <c r="G3" s="6" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="11" r="H3">
+      <c r="H3" s="11" t="s">
         <v>22</v>
       </c>
-      <c s="1" r="I3"/>
-    </row>
-    <row r="4">
-      <c t="s" s="3" r="A4">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="2" r="B4">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="2" r="C4">
+      <c r="C4" s="2" t="s">
         <v>24</v>
       </c>
-      <c t="s" s="2" r="D4">
+      <c r="D4" s="2" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="13" r="E4">
+      <c r="E4" s="13" t="s">
         <v>26</v>
       </c>
-      <c t="s" s="13" r="F4">
+      <c r="F4" s="13" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="6" r="G4">
+      <c r="G4" s="6" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="4" r="H4">
+      <c r="H4" s="4" t="s">
         <v>15</v>
       </c>
-      <c s="1" r="I4"/>
-    </row>
-    <row r="5">
-      <c t="s" s="3" r="A5">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
-      <c t="s" s="12" r="B5">
+      <c r="B5" s="12" t="s">
         <v>29</v>
       </c>
-      <c t="s" s="2" r="C5">
+      <c r="C5" s="2" t="s">
         <v>30</v>
       </c>
-      <c t="s" s="2" r="D5">
+      <c r="D5" s="2" t="s">
         <v>31</v>
       </c>
-      <c s="13" r="E5">
+      <c r="E5" s="13">
         <v>4</v>
       </c>
-      <c t="s" s="13" r="F5">
+      <c r="F5" s="13" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="6" r="G5">
+      <c r="G5" s="6" t="s">
         <v>33</v>
       </c>
-      <c t="s" s="11" r="H5">
+      <c r="H5" s="11" t="s">
         <v>34</v>
       </c>
-      <c s="1" r="I5"/>
-    </row>
-    <row r="6">
-      <c t="s" s="3" r="A6">
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="12" r="B6">
+      <c r="B6" s="12" t="s">
         <v>29</v>
       </c>
-      <c t="s" s="2" r="C6">
+      <c r="C6" s="2" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="2" r="D6">
+      <c r="D6" s="2" t="s">
         <v>37</v>
       </c>
-      <c s="13" r="E6">
+      <c r="E6" s="13">
         <v>4</v>
       </c>
-      <c t="s" s="13" r="F6">
+      <c r="F6" s="13" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="13" r="G6">
+      <c r="G6" s="13" t="s">
         <v>38</v>
       </c>
-      <c t="s" s="11" r="H6">
+      <c r="H6" s="11" t="s">
         <v>39</v>
       </c>
-      <c s="1" r="I6"/>
-    </row>
-    <row r="7">
-      <c t="s" s="3" r="A7">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="12" r="B7">
+      <c r="B7" s="12" t="s">
         <v>29</v>
       </c>
-      <c t="s" s="2" r="C7">
+      <c r="C7" s="2" t="s">
         <v>41</v>
       </c>
-      <c t="s" s="2" r="D7">
+      <c r="D7" s="2" t="s">
         <v>42</v>
       </c>
-      <c s="13" r="E7">
+      <c r="E7" s="13">
         <v>4</v>
       </c>
-      <c t="s" s="13" r="F7">
+      <c r="F7" s="13" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="13" r="G7">
+      <c r="G7" s="13" t="s">
         <v>43</v>
       </c>
-      <c t="s" s="11" r="H7">
+      <c r="H7" s="11" t="s">
         <v>44</v>
       </c>
-      <c s="1" r="I7"/>
-    </row>
-    <row r="8">
-      <c t="s" s="3" r="A8">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>45</v>
       </c>
-      <c t="s" s="2" r="B8">
+      <c r="B8" s="2" t="s">
         <v>46</v>
       </c>
-      <c t="s" s="2" r="C8">
+      <c r="C8" s="2" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="2" r="D8">
+      <c r="D8" s="2" t="s">
         <v>48</v>
       </c>
-      <c s="13" r="E8">
+      <c r="E8" s="13">
         <v>29</v>
       </c>
-      <c t="s" s="13" r="F8">
+      <c r="F8" s="13" t="s">
         <v>49</v>
       </c>
-      <c t="s" s="13" r="G8">
+      <c r="G8" s="13" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="11" r="H8">
+      <c r="H8" s="11" t="s">
         <v>51</v>
       </c>
-      <c s="1" r="I8"/>
-    </row>
-    <row r="9">
-      <c t="s" s="3" r="A9">
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="2" r="B9">
+      <c r="B9" s="2" t="s">
         <v>46</v>
       </c>
-      <c t="s" s="2" r="C9">
+      <c r="C9" s="2" t="s">
         <v>53</v>
       </c>
-      <c t="s" s="2" r="D9">
+      <c r="D9" s="2" t="s">
         <v>54</v>
       </c>
-      <c t="s" s="13" r="E9">
+      <c r="E9" s="13" t="s">
         <v>55</v>
       </c>
-      <c t="s" s="13" r="F9">
+      <c r="F9" s="13" t="s">
         <v>56</v>
       </c>
-      <c t="s" s="13" r="G9">
+      <c r="G9" s="13" t="s">
         <v>57</v>
       </c>
-      <c t="s" s="11" r="H9">
+      <c r="H9" s="11" t="s">
         <v>58</v>
       </c>
-      <c s="1" r="I9"/>
-    </row>
-    <row r="10">
-      <c t="s" s="3" r="A10">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>59</v>
       </c>
-      <c t="s" s="9" r="B10">
+      <c r="B10" s="9" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="2" r="C10">
+      <c r="C10" s="2" t="s">
         <v>60</v>
       </c>
-      <c t="s" s="2" r="D10">
+      <c r="D10" s="2" t="s">
         <v>61</v>
       </c>
-      <c s="13" r="E10">
+      <c r="E10" s="13">
         <v>4</v>
       </c>
-      <c t="s" s="13" r="F10">
+      <c r="F10" s="13" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="13" r="G10">
+      <c r="G10" s="13" t="s">
         <v>62</v>
       </c>
-      <c t="s" s="11" r="H10">
+      <c r="H10" s="11" t="s">
         <v>63</v>
       </c>
-      <c s="1" r="I10"/>
-    </row>
-    <row r="11">
-      <c t="s" s="3" r="A11">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>64</v>
       </c>
-      <c t="s" s="2" r="B11">
+      <c r="B11" s="2" t="s">
         <v>46</v>
       </c>
-      <c t="s" s="2" r="C11">
+      <c r="C11" s="2" t="s">
         <v>65</v>
       </c>
-      <c t="s" s="2" r="D11">
+      <c r="D11" s="2" t="s">
         <v>66</v>
       </c>
-      <c s="13" r="E11">
+      <c r="E11" s="13">
         <v>103</v>
       </c>
-      <c t="s" s="13" r="F11">
+      <c r="F11" s="13" t="s">
         <v>67</v>
       </c>
-      <c t="s" s="6" r="G11">
+      <c r="G11" s="6" t="s">
         <v>68</v>
       </c>
-      <c s="11" r="H11"/>
-      <c s="1" r="I11"/>
-    </row>
-    <row r="12">
-      <c t="s" s="3" r="A12">
+      <c r="H11" s="11"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>69</v>
       </c>
-      <c t="s" s="9" r="B12">
+      <c r="B12" s="9" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="2" r="C12">
+      <c r="C12" s="2" t="s">
         <v>70</v>
       </c>
-      <c t="s" s="2" r="D12">
+      <c r="D12" s="2" t="s">
         <v>71</v>
       </c>
-      <c s="13" r="E12">
+      <c r="E12" s="13">
         <v>4</v>
       </c>
-      <c t="s" s="13" r="F12">
+      <c r="F12" s="13" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="13" r="G12">
+      <c r="G12" s="13" t="s">
         <v>72</v>
       </c>
-      <c t="s" s="11" r="H12">
+      <c r="H12" s="11" t="s">
         <v>73</v>
       </c>
-      <c s="1" r="I12"/>
-    </row>
-    <row r="13">
-      <c t="s" s="3" r="A13">
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>74</v>
       </c>
-      <c t="s" s="2" r="B13">
+      <c r="B13" s="2" t="s">
         <v>46</v>
       </c>
-      <c t="s" s="2" r="C13">
+      <c r="C13" s="2" t="s">
         <v>75</v>
       </c>
-      <c t="s" s="2" r="D13">
+      <c r="D13" s="2" t="s">
         <v>76</v>
       </c>
-      <c t="s" s="13" r="E13">
+      <c r="E13" s="13" t="s">
         <v>77</v>
       </c>
-      <c t="s" s="13" r="F13">
+      <c r="F13" s="13" t="s">
         <v>49</v>
       </c>
-      <c t="s" s="13" r="G13">
+      <c r="G13" s="13" t="s">
         <v>78</v>
       </c>
-      <c t="s" s="11" r="H13">
+      <c r="H13" s="11" t="s">
         <v>79</v>
       </c>
-      <c s="1" r="I13"/>
-    </row>
-    <row r="14">
-      <c t="s" s="3" r="A14">
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>80</v>
       </c>
-      <c t="s" s="2" r="B14">
+      <c r="B14" s="2" t="s">
         <v>81</v>
       </c>
-      <c t="s" s="2" r="C14">
+      <c r="C14" s="2" t="s">
         <v>82</v>
       </c>
-      <c t="s" s="2" r="D14">
+      <c r="D14" s="2" t="s">
         <v>83</v>
       </c>
-      <c t="s" s="13" r="E14">
+      <c r="E14" s="13" t="s">
         <v>84</v>
       </c>
-      <c t="s" s="13" r="F14">
+      <c r="F14" s="13" t="s">
         <v>49</v>
       </c>
-      <c t="s" s="13" r="G14">
+      <c r="G14" s="13" t="s">
         <v>85</v>
       </c>
-      <c t="s" s="11" r="H14">
+      <c r="H14" s="11" t="s">
         <v>86</v>
       </c>
-      <c s="1" r="I14"/>
-    </row>
-    <row r="15">
-      <c t="s" s="3" r="A15">
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>87</v>
       </c>
-      <c t="s" s="9" r="B15">
+      <c r="B15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>88</v>
       </c>
-      <c t="s" s="2" r="C15">
+      <c r="D15" s="2" t="s">
         <v>89</v>
       </c>
-      <c t="s" s="2" r="D15">
+      <c r="E15" s="13">
+        <v>37</v>
+      </c>
+      <c r="F15" s="13" t="s">
         <v>90</v>
       </c>
-      <c s="13" r="E15">
-        <v>37</v>
-      </c>
-      <c t="s" s="13" r="F15">
+      <c r="G15" s="6" t="s">
         <v>91</v>
       </c>
-      <c t="s" s="6" r="G15">
+      <c r="H15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>92</v>
       </c>
-      <c t="s" s="4" r="H15">
+      <c r="B16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="13">
+        <v>250</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>15</v>
       </c>
-      <c s="1" r="I15"/>
-    </row>
-    <row r="16">
-      <c t="s" s="3" r="A16">
-        <v>93</v>
-      </c>
-      <c t="s" s="2" r="B16">
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>81</v>
       </c>
-      <c t="s" s="2" r="C16">
-        <v>94</v>
-      </c>
-      <c t="s" s="2" r="D16">
-        <v>95</v>
-      </c>
-      <c s="13" r="E16">
-        <v>250</v>
-      </c>
-      <c t="s" s="13" r="F16">
+      <c r="C17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="13">
+        <v>7</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="13">
         <v>13</v>
       </c>
-      <c t="s" s="6" r="G16">
-        <v>96</v>
-      </c>
-      <c t="s" s="4" r="H16">
-        <v>15</v>
-      </c>
-      <c s="1" r="I16"/>
-    </row>
-    <row r="17">
-      <c t="s" s="3" r="A17">
-        <v>97</v>
-      </c>
-      <c t="s" s="2" r="B17">
-        <v>81</v>
-      </c>
-      <c t="s" s="2" r="C17">
-        <v>98</v>
-      </c>
-      <c t="s" s="2" r="D17">
-        <v>99</v>
-      </c>
-      <c s="13" r="E17">
-        <v>7</v>
-      </c>
-      <c t="s" s="13" r="F17">
-        <v>20</v>
-      </c>
-      <c t="s" s="13" r="G17">
-        <v>100</v>
-      </c>
-      <c t="s" s="11" r="H17">
-        <v>101</v>
-      </c>
-      <c s="1" r="I17"/>
-    </row>
-    <row r="18">
-      <c t="s" s="3" r="A18">
-        <v>102</v>
-      </c>
-      <c t="s" s="2" r="B18">
-        <v>81</v>
-      </c>
-      <c t="s" s="2" r="C18">
-        <v>103</v>
-      </c>
-      <c t="s" s="2" r="D18">
+      <c r="F18" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="13" t="s">
         <v>104</v>
       </c>
-      <c s="13" r="E18">
+      <c r="H18" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="13">
+        <v>4</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="13">
+        <v>4</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="13">
+        <v>4</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D24" s="5"/>
+      <c r="E24" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D25" s="5"/>
+      <c r="E25" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="13" r="F18">
-        <v>56</v>
-      </c>
-      <c t="s" s="13" r="G18">
-        <v>105</v>
-      </c>
-      <c t="s" s="11" r="H18">
-        <v>106</v>
-      </c>
-      <c s="1" r="I18"/>
-    </row>
-    <row r="19">
-      <c t="s" s="3" r="A19">
-        <v>107</v>
-      </c>
-      <c t="s" s="12" r="B19">
-        <v>108</v>
-      </c>
-      <c t="s" s="2" r="C19">
-        <v>109</v>
-      </c>
-      <c t="s" s="2" r="D19">
-        <v>110</v>
-      </c>
-      <c s="13" r="E19">
-        <v>4</v>
-      </c>
-      <c t="s" s="13" r="F19">
-        <v>32</v>
-      </c>
-      <c t="s" s="13" r="G19">
-        <v>111</v>
-      </c>
-      <c t="s" s="11" r="H19">
-        <v>112</v>
-      </c>
-      <c s="1" r="I19"/>
-    </row>
-    <row r="20">
-      <c t="s" s="3" r="A20">
-        <v>113</v>
-      </c>
-      <c t="s" s="2" r="B20">
-        <v>108</v>
-      </c>
-      <c t="s" s="2" r="C20">
-        <v>114</v>
-      </c>
-      <c t="s" s="2" r="D20">
-        <v>115</v>
-      </c>
-      <c s="13" r="E20">
-        <v>4</v>
-      </c>
-      <c t="s" s="13" r="F20">
-        <v>32</v>
-      </c>
-      <c t="s" s="13" r="G20">
-        <v>116</v>
-      </c>
-      <c t="s" s="11" r="H20">
-        <v>117</v>
-      </c>
-      <c s="1" r="I20"/>
-    </row>
-    <row r="21">
-      <c t="s" s="3" r="A21">
-        <v>118</v>
-      </c>
-      <c t="s" s="2" r="B21">
-        <v>108</v>
-      </c>
-      <c t="s" s="2" r="C21">
-        <v>119</v>
-      </c>
-      <c t="s" s="2" r="D21">
-        <v>120</v>
-      </c>
-      <c s="13" r="E21">
-        <v>4</v>
-      </c>
-      <c t="s" s="13" r="F21">
-        <v>32</v>
-      </c>
-      <c t="s" s="13" r="G21">
-        <v>121</v>
-      </c>
-      <c t="s" s="11" r="H21">
-        <v>122</v>
-      </c>
-      <c s="1" r="I21"/>
-    </row>
-    <row r="22">
-      <c s="7" r="A22"/>
-      <c s="7" r="B22"/>
-      <c s="7" r="C22"/>
-      <c s="7" r="D22"/>
-      <c s="7" r="E22"/>
-      <c s="7" r="F22"/>
-      <c s="7" r="G22"/>
-      <c s="7" r="H22"/>
-    </row>
-    <row r="23">
-      <c s="8" r="E23"/>
-      <c s="8" r="F23"/>
-    </row>
-    <row r="24">
-      <c s="5" r="D24"/>
-      <c t="s" s="10" r="E24">
-        <v>123</v>
-      </c>
-      <c t="s" s="10" r="F24">
-        <v>124</v>
-      </c>
-      <c s="1" r="G24"/>
-    </row>
-    <row r="25">
-      <c s="5" r="D25"/>
-      <c t="s" s="3" r="E25">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D26" s="5"/>
+      <c r="E26" s="3" t="s">
         <v>125</v>
       </c>
-      <c t="s" s="2" r="F25">
+      <c r="F26" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D27" s="5"/>
+      <c r="E27" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>13</v>
       </c>
-      <c s="1" r="G25"/>
-    </row>
-    <row r="26">
-      <c s="5" r="D26"/>
-      <c t="s" s="3" r="E26">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D28" s="5"/>
+      <c r="E28" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D29" s="5"/>
+      <c r="E29" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D30" s="5"/>
+      <c r="E30" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>126</v>
       </c>
-      <c t="s" s="2" r="F26">
-        <v>127</v>
-      </c>
-      <c s="1" r="G26"/>
-    </row>
-    <row r="27">
-      <c s="5" r="D27"/>
-      <c t="s" s="3" r="E27">
-        <v>128</v>
-      </c>
-      <c t="s" s="2" r="F27">
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D31" s="5"/>
+      <c r="E31" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>13</v>
       </c>
-      <c s="1" r="G27"/>
-    </row>
-    <row r="28">
-      <c s="5" r="D28"/>
-      <c t="s" s="3" r="E28">
-        <v>129</v>
-      </c>
-      <c t="s" s="2" r="F28">
-        <v>91</v>
-      </c>
-      <c s="1" r="G28"/>
-    </row>
-    <row r="29">
-      <c s="5" r="D29"/>
-      <c t="s" s="3" r="E29">
-        <v>130</v>
-      </c>
-      <c t="s" s="2" r="F29">
-        <v>67</v>
-      </c>
-      <c s="1" r="G29"/>
-    </row>
-    <row r="30">
-      <c s="5" r="D30"/>
-      <c t="s" s="3" r="E30">
-        <v>131</v>
-      </c>
-      <c t="s" s="2" r="F30">
-        <v>127</v>
-      </c>
-      <c s="1" r="G30"/>
-    </row>
-    <row r="31">
-      <c s="5" r="D31"/>
-      <c t="s" s="3" r="E31">
-        <v>132</v>
-      </c>
-      <c t="s" s="2" r="F31">
-        <v>13</v>
-      </c>
-      <c s="1" r="G31"/>
-    </row>
-    <row r="32">
-      <c s="7" r="E32"/>
-      <c s="7" r="F32"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
asigne las ips de las 3 redes del frame relay en las tablas. ahora cambio los configs
</commit_message>
<xml_diff>
--- a/ tp-distribuidos-grupo3/Tabla de subredes - Subnetting.xlsx
+++ b/ tp-distribuidos-grupo3/Tabla de subredes - Subnetting.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="540" windowWidth="18615" windowHeight="5835"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="140">
   <si>
     <t>Red</t>
   </si>
@@ -64,27 +64,18 @@
     <t>Completo</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>Enlace!</t>
   </si>
   <si>
     <t>Bianchi</t>
   </si>
   <si>
-    <t>R1-R12-R13 (FrameRelay)</t>
-  </si>
-  <si>
     <t>/29</t>
   </si>
   <si>
     <t>172.143.0.64</t>
   </si>
   <si>
-    <t>Quedan .72-.255 = 183</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -410,13 +401,46 @@
   </si>
   <si>
     <t>10.118.5.0 (A)</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>R1-R13 (FrameRelay)</t>
+  </si>
+  <si>
+    <t>R12-R13 (FrameRelay)</t>
+  </si>
+  <si>
+    <t>R1-R12 (FrameRelay)</t>
+  </si>
+  <si>
+    <t>172.143.0.68</t>
+  </si>
+  <si>
+    <t>172.143.0.72</t>
+  </si>
+  <si>
+    <t>sigue b2</t>
+  </si>
+  <si>
+    <t>sigue b3</t>
+  </si>
+  <si>
+    <t>Quedan .76-.255 = 179</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -458,6 +482,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -656,7 +686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -698,6 +728,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1000,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1072,564 +1114,594 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="13">
+        <v>4</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="13">
-        <v>5</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>22</v>
+      <c r="H3" s="17" t="s">
+        <v>137</v>
       </c>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>130</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>26</v>
+        <v>132</v>
+      </c>
+      <c r="E4" s="13">
+        <v>4</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>15</v>
+        <v>29</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="A5" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="15"/>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>133</v>
       </c>
       <c r="E5" s="13">
         <v>4</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>34</v>
+        <v>29</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>139</v>
       </c>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>29</v>
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="13">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E7" s="13">
         <v>4</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>43</v>
+        <v>29</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>32</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E8" s="13">
+        <v>4</v>
+      </c>
+      <c r="F8" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="13" t="s">
-        <v>49</v>
-      </c>
       <c r="G8" s="13" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>55</v>
+        <v>39</v>
+      </c>
+      <c r="E9" s="13">
+        <v>4</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>17</v>
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="E10" s="13">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="13">
-        <v>103</v>
+        <v>51</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="11"/>
+        <v>53</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>55</v>
+      </c>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E12" s="13">
         <v>4</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>77</v>
+        <v>63</v>
+      </c>
+      <c r="E13" s="13">
+        <v>103</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>79</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="11"/>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>81</v>
+        <v>66</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>84</v>
+        <v>68</v>
+      </c>
+      <c r="E14" s="13">
+        <v>4</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15" s="13">
-        <v>37</v>
+        <v>73</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>15</v>
+        <v>46</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E16" s="13">
-        <v>250</v>
-      </c>
       <c r="F16" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>15</v>
+        <v>46</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E17" s="13">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E18" s="13">
+        <v>250</v>
+      </c>
+      <c r="F18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>105</v>
+      <c r="G18" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>107</v>
+        <v>93</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="E19" s="13">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E20" s="13">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="E21" s="13">
         <v>4</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G21" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="13">
+        <v>4</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="13">
+        <v>4</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D26" s="5"/>
+      <c r="E26" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>120</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D24" s="5"/>
-      <c r="E24" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D25" s="5"/>
-      <c r="E25" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D26" s="5"/>
-      <c r="E26" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D27" s="5"/>
       <c r="E27" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>13</v>
@@ -1639,48 +1711,69 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D28" s="5"/>
       <c r="E28" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D29" s="5"/>
       <c r="E29" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D30" s="5"/>
       <c r="E30" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>126</v>
+        <v>87</v>
       </c>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D31" s="5"/>
       <c r="E31" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D32" s="5"/>
+      <c r="E32" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D33" s="5"/>
+      <c r="E33" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>